<commit_message>
Fix bug spécialisation château
Quand le province perdait son statut de capitale, la cité fortifiée même
construite n'apparaissait plus.
La spécialisation féodale se fait uniquement  par event.

Correction du tableau des features (aucune fonctionnalités de Xylo n'a
été reprise)
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -863,7 +863,7 @@
   <dimension ref="A1:I39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1292,8 +1292,8 @@
       <c r="E17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>7</v>
+      <c r="F17" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>51</v>
@@ -1317,8 +1317,8 @@
       <c r="E18" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F18" s="7" t="s">
-        <v>12</v>
+      <c r="F18" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Maj tableau des features
Des features de Xylo ont été rajouté ainsi qu'une feature de
modification de l'autorité religieuse
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="116">
   <si>
     <t>Catégorie</t>
   </si>
@@ -348,6 +348,30 @@
   </si>
   <si>
     <t>Events fantastiques</t>
+  </si>
+  <si>
+    <t>Modification autorité religieuse</t>
+  </si>
+  <si>
+    <t>Certaines actions ont désormais des effets sur l'autorité religieuse</t>
+  </si>
+  <si>
+    <t>Forestier</t>
+  </si>
+  <si>
+    <t>Le forestier vous permet de gérer votre forêt</t>
+  </si>
+  <si>
+    <t>On peut éviter de nommer le forestier pour éviter les problèmes …</t>
+  </si>
+  <si>
+    <t>Spécialisation forêt</t>
+  </si>
+  <si>
+    <t>Les forêts se spécialisent en exploitation, chasse, …</t>
+  </si>
+  <si>
+    <t>On peut ajouter toujours plus de flavour events</t>
   </si>
 </sst>
 </file>
@@ -860,10 +884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,26 +1278,24 @@
         <v>44</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>110</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>48</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="15"/>
       <c r="I16" s="6"/>
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1281,22 +1303,22 @@
         <v>44</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>49</v>
+        <v>113</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>51</v>
+        <v>114</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="H17" s="15"/>
       <c r="I17" s="6"/>
@@ -1306,24 +1328,26 @@
         <v>44</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>12</v>
+        <v>46</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F18" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="15"/>
+      <c r="G18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>48</v>
+      </c>
       <c r="I18" s="6"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1331,71 +1355,71 @@
         <v>44</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>101</v>
+        <v>49</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G19" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="H19" s="15"/>
       <c r="I19" s="6"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12" t="s">
-        <v>54</v>
+      <c r="A20" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="H20" s="15"/>
       <c r="I20" s="6"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12" t="s">
-        <v>54</v>
+      <c r="A21" s="11" t="s">
+        <v>44</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>48</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" s="5"/>
       <c r="H21" s="15"/>
       <c r="I21" s="6"/>
     </row>
@@ -1404,26 +1428,24 @@
         <v>54</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="H22" s="16" t="s">
-        <v>48</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H22" s="15"/>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1431,26 +1453,24 @@
         <v>54</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>67</v>
-      </c>
+      <c r="E23" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="15"/>
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1458,25 +1478,25 @@
         <v>54</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>71</v>
+        <v>61</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F24" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>48</v>
       </c>
       <c r="I24" s="6"/>
     </row>
@@ -1485,53 +1505,53 @@
         <v>54</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="20" t="s">
-        <v>100</v>
+        <v>65</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>76</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>54</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F26" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H26" s="15"/>
+        <v>69</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>71</v>
+      </c>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1539,120 +1559,197 @@
         <v>54</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>81</v>
+        <v>73</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H27" s="15"/>
-      <c r="I27" s="6"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="H27" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>104</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" s="15"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="19" t="s">
+      <c r="B29" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H29" s="15"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D30" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="18" t="s">
+      <c r="D32" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="2" t="s">
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
+    <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B38" s="14" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="2" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B40" s="14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="21" t="s">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B42" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1664,14 +1761,14 @@
     <hyperlink ref="H11" r:id="rId4" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052712346"/>
     <hyperlink ref="G13" r:id="rId5" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052713286"/>
     <hyperlink ref="G14" r:id="rId6" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052727226"/>
-    <hyperlink ref="H16" r:id="rId7" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052708015"/>
-    <hyperlink ref="G17" r:id="rId8" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052657380"/>
-    <hyperlink ref="G18" r:id="rId9" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052648061"/>
-    <hyperlink ref="G21" r:id="rId10" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052705143"/>
-    <hyperlink ref="H22" r:id="rId11" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052704582"/>
-    <hyperlink ref="H25" r:id="rId12" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052647414"/>
-    <hyperlink ref="I25" r:id="rId13" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/page-6"/>
-    <hyperlink ref="G26" r:id="rId14" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052721481"/>
+    <hyperlink ref="H18" r:id="rId7" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052708015"/>
+    <hyperlink ref="G19" r:id="rId8" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052657380"/>
+    <hyperlink ref="G20" r:id="rId9" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052648061"/>
+    <hyperlink ref="G23" r:id="rId10" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052705143"/>
+    <hyperlink ref="H24" r:id="rId11" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052704582"/>
+    <hyperlink ref="H27" r:id="rId12" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052647414"/>
+    <hyperlink ref="I27" r:id="rId13" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/page-6"/>
+    <hyperlink ref="G28" r:id="rId14" display="http://forum.reseau-js.com/topic/87034-mod-les-trois-tours-l3t/?p=1052721481"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>

</xml_diff>